<commit_message>
Added Hungama POC project
</commit_message>
<xml_diff>
--- a/RestAssuredExample/test-data/testData.xlsx
+++ b/RestAssuredExample/test-data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14790" windowHeight="6345"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>JSON Body File Name</t>
   </si>
   <si>
-    <t>http://172.16.2.154:9090/task_manager/v1/</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>false,You are successfully registered</t>
+  </si>
+  <si>
+    <t>http://172.16.2.96:9090/task_manager/v1/</t>
   </si>
 </sst>
 </file>
@@ -549,8 +549,8 @@
   <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V3" sqref="V3"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -558,7 +558,8 @@
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="40.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -624,10 +625,10 @@
         <v>21</v>
       </c>
       <c r="P1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R1" t="s">
         <v>14</v>
@@ -653,319 +654,319 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>27</v>
       </c>
-      <c r="R2" t="s">
-        <v>28</v>
-      </c>
       <c r="S2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="T2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>26</v>
       </c>
-      <c r="M3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" t="s">
-        <v>27</v>
-      </c>
       <c r="R3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U3" t="s">
+        <v>51</v>
+      </c>
+      <c r="V3" t="s">
         <v>52</v>
-      </c>
-      <c r="V3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" t="s">
         <v>23</v>
       </c>
-      <c r="J4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>26</v>
       </c>
-      <c r="M4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" t="s">
-        <v>27</v>
-      </c>
       <c r="R4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" t="s">
         <v>34</v>
       </c>
-      <c r="S4" t="s">
-        <v>35</v>
-      </c>
       <c r="T4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U4" t="s">
+        <v>53</v>
+      </c>
+      <c r="V4" t="s">
         <v>54</v>
-      </c>
-      <c r="V4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>24</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>25</v>
       </c>
-      <c r="L5" t="s">
-        <v>26</v>
-      </c>
       <c r="M5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:22">
       <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>24</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>25</v>
       </c>
-      <c r="L6" t="s">
-        <v>26</v>
-      </c>
       <c r="M6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T6" t="s">
+        <v>62</v>
+      </c>
+      <c r="U6" t="s">
         <v>63</v>
       </c>
-      <c r="U6" t="s">
-        <v>64</v>
-      </c>
       <c r="V6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:22">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R7" t="s">
         <v>41</v>
       </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" t="s">
-        <v>27</v>
-      </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>42</v>
       </c>
-      <c r="S7" t="s">
-        <v>43</v>
-      </c>
       <c r="T7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:22">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
       <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
         <v>23</v>
       </c>
-      <c r="H8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>24</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>25</v>
       </c>
-      <c r="L8" t="s">
-        <v>26</v>
-      </c>
       <c r="M8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>